<commit_message>
add DAC to Contract
</commit_message>
<xml_diff>
--- a/easylight/doc/Tarifa_Alto_Consumo.xlsx
+++ b/easylight/doc/Tarifa_Alto_Consumo.xlsx
@@ -78,7 +78,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -99,6 +99,11 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="13"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -121,7 +126,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -264,13 +269,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -298,9 +318,6 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -313,7 +330,16 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -337,6 +363,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1459,1346 +1486,1642 @@
       <c r="F2" s="8">
         <v>3.468</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" ht="20.7" customHeight="1">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="10">
         <v>1</v>
       </c>
       <c r="C3" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>97.01000000000001</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>4.193</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="12">
         <v>3.601</v>
       </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" ht="20.7" customHeight="1">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>1</v>
       </c>
       <c r="C4" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>99.95</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <v>4.528</v>
       </c>
-      <c r="F4" s="13">
+      <c r="F4" s="12">
         <v>3.889</v>
       </c>
-      <c r="G4" s="14"/>
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" ht="20.7" customHeight="1">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>1</v>
       </c>
       <c r="C5" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>100.55</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="9">
         <v>4.462</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="12">
         <v>3.833</v>
       </c>
-      <c r="G5" s="14"/>
+      <c r="G5" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" ht="20.7" customHeight="1">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>1</v>
       </c>
       <c r="C6" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>99.84</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>4.246</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="12">
         <v>3.647</v>
       </c>
-      <c r="G6" s="14"/>
+      <c r="G6" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" ht="20.7" customHeight="1">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="10">
         <v>1</v>
       </c>
       <c r="C7" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>98.70999999999999</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <v>4.232</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="12">
         <v>3.635</v>
       </c>
-      <c r="G7" s="14"/>
+      <c r="G7" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" ht="20.7" customHeight="1">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>1</v>
       </c>
       <c r="C8" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>98.86</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="9">
         <v>4.225</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>3.629</v>
       </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" ht="20.7" customHeight="1">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <v>8</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9" s="10">
         <v>1</v>
       </c>
       <c r="C9" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>98</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>4.153</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <v>3.567</v>
       </c>
-      <c r="G9" s="14"/>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" ht="20.7" customHeight="1">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>1</v>
       </c>
       <c r="C10" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>97.51000000000001</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>4.115</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <v>3.535</v>
       </c>
-      <c r="G10" s="14"/>
+      <c r="G10" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" ht="20.7" customHeight="1">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <v>10</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11" s="10">
         <v>1</v>
       </c>
       <c r="C11" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>97.70999999999999</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>4.141</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <v>3.557</v>
       </c>
-      <c r="G11" s="14"/>
+      <c r="G11" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" ht="20.7" customHeight="1">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12" s="10">
         <v>1</v>
       </c>
       <c r="C12" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="D12" s="13">
+        <v>98.04000000000001</v>
+      </c>
+      <c r="E12" s="12">
+        <v>4.201</v>
+      </c>
+      <c r="F12" s="14">
+        <v>3.61</v>
+      </c>
+      <c r="G12" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" ht="20.7" customHeight="1">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <v>12</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="10">
         <v>1</v>
       </c>
       <c r="C13" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="12">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" ht="20.7" customHeight="1">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <v>13</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="10">
         <v>2</v>
       </c>
       <c r="C14" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="11">
         <v>95.67</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="12">
         <v>4.401</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <v>3.468</v>
       </c>
-      <c r="G14" s="13"/>
+      <c r="G14" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" ht="20.7" customHeight="1">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <v>14</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15" s="10">
         <v>2</v>
       </c>
       <c r="C15" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="11">
         <v>97.01000000000001</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="12">
         <v>4.57</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="12">
         <v>3.601</v>
       </c>
-      <c r="G15" s="13"/>
+      <c r="G15" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" ht="20.7" customHeight="1">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16" s="10">
         <v>2</v>
       </c>
       <c r="C16" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>99.95</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="12">
         <v>4.935</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
         <v>3.889</v>
       </c>
-      <c r="G16" s="13"/>
+      <c r="G16" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" ht="20.7" customHeight="1">
-      <c r="A17" s="10">
+      <c r="A17" s="9">
         <v>16</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="10">
         <v>2</v>
       </c>
       <c r="C17" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="11">
         <v>100.55</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="12">
         <v>4.863</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="12">
         <v>3.833</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" ht="20.7" customHeight="1">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <v>17</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="10">
         <v>2</v>
       </c>
       <c r="C18" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <v>99.84</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="12">
         <v>4.628</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <v>3.647</v>
       </c>
-      <c r="G18" s="13"/>
+      <c r="G18" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" ht="20.7" customHeight="1">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <v>18</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19" s="10">
         <v>2</v>
       </c>
       <c r="C19" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="11">
         <v>98.70999999999999</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="12">
         <v>4.612</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <v>3.635</v>
       </c>
-      <c r="G19" s="13"/>
+      <c r="G19" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" ht="20.7" customHeight="1">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <v>19</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20" s="10">
         <v>2</v>
       </c>
       <c r="C20" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="11">
         <v>98.86</v>
       </c>
-      <c r="E20" s="13">
+      <c r="E20" s="12">
         <v>4.605</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <v>3.629</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="21" ht="20.7" customHeight="1">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <v>20</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21" s="10">
         <v>2</v>
       </c>
       <c r="C21" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21" s="11">
         <v>98</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="12">
         <v>4.526</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <v>3.567</v>
       </c>
-      <c r="G21" s="13"/>
+      <c r="G21" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" ht="20.7" customHeight="1">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <v>21</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22" s="10">
         <v>2</v>
       </c>
       <c r="C22" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="11">
         <v>97.51000000000001</v>
       </c>
-      <c r="E22" s="13">
+      <c r="E22" s="12">
         <v>4.485</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="12">
         <v>3.535</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" ht="20.7" customHeight="1">
-      <c r="A23" s="10">
+      <c r="A23" s="9">
         <v>22</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23" s="10">
         <v>2</v>
       </c>
       <c r="C23" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D23" s="12">
+      <c r="D23" s="11">
         <v>97.70999999999999</v>
       </c>
-      <c r="E23" s="13">
+      <c r="E23" s="12">
         <v>4.513</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="12">
         <v>3.557</v>
       </c>
-      <c r="G23" s="13"/>
+      <c r="G23" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="24" ht="20.7" customHeight="1">
-      <c r="A24" s="10">
+      <c r="A24" s="9">
         <v>23</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24" s="10">
         <v>2</v>
       </c>
       <c r="C24" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
+      <c r="D24" s="15">
+        <v>98.04000000000001</v>
+      </c>
+      <c r="E24" s="11">
+        <v>4.58</v>
+      </c>
+      <c r="F24" s="12">
+        <v>3.61</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="25" ht="20.7" customHeight="1">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <v>24</v>
       </c>
-      <c r="B25" s="11">
+      <c r="B25" s="10">
         <v>2</v>
       </c>
       <c r="C25" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="D25" s="15">
+        <v>0</v>
+      </c>
+      <c r="E25" s="15">
+        <v>0</v>
+      </c>
+      <c r="F25" s="11">
+        <v>0</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="26" ht="20.7" customHeight="1">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <v>25</v>
       </c>
-      <c r="B26" s="11">
+      <c r="B26" s="10">
         <v>3</v>
       </c>
       <c r="C26" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26" s="11">
         <v>95.67</v>
       </c>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13">
+      <c r="E26" s="12">
+        <v>0</v>
+      </c>
+      <c r="F26" s="12">
+        <v>0</v>
+      </c>
+      <c r="G26" s="12">
         <v>4.156</v>
       </c>
     </row>
     <row r="27" ht="20.7" customHeight="1">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <v>26</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27" s="10">
         <v>3</v>
       </c>
       <c r="C27" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27" s="11">
         <v>97.01000000000001</v>
       </c>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13">
+      <c r="E27" s="12">
+        <v>0</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
+      </c>
+      <c r="G27" s="12">
         <v>4.315</v>
       </c>
     </row>
     <row r="28" ht="20.7" customHeight="1">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <v>27</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28" s="10">
         <v>3</v>
       </c>
       <c r="C28" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="11">
         <v>99.95</v>
       </c>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13">
+      <c r="E28" s="12">
+        <v>0</v>
+      </c>
+      <c r="F28" s="12">
+        <v>0</v>
+      </c>
+      <c r="G28" s="12">
         <v>4.66</v>
       </c>
     </row>
     <row r="29" ht="20.7" customHeight="1">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <v>28</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29" s="10">
         <v>3</v>
       </c>
       <c r="C29" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29" s="11">
         <v>100.55</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13">
+      <c r="E29" s="12">
+        <v>0</v>
+      </c>
+      <c r="F29" s="12">
+        <v>0</v>
+      </c>
+      <c r="G29" s="12">
         <v>4.592</v>
       </c>
     </row>
     <row r="30" ht="20.7" customHeight="1">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <v>29</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30" s="10">
         <v>3</v>
       </c>
       <c r="C30" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="11">
         <v>99.84</v>
       </c>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13">
+      <c r="E30" s="12">
+        <v>0</v>
+      </c>
+      <c r="F30" s="12">
+        <v>0</v>
+      </c>
+      <c r="G30" s="12">
         <v>4.37</v>
       </c>
     </row>
     <row r="31" ht="20.7" customHeight="1">
-      <c r="A31" s="10">
+      <c r="A31" s="9">
         <v>30</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31" s="10">
         <v>3</v>
       </c>
       <c r="C31" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="11">
         <v>98.70999999999999</v>
       </c>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13">
+      <c r="E31" s="12">
+        <v>0</v>
+      </c>
+      <c r="F31" s="12">
+        <v>0</v>
+      </c>
+      <c r="G31" s="12">
         <v>4.355</v>
       </c>
     </row>
     <row r="32" ht="20.7" customHeight="1">
-      <c r="A32" s="10">
+      <c r="A32" s="9">
         <v>31</v>
       </c>
-      <c r="B32" s="11">
+      <c r="B32" s="10">
         <v>3</v>
       </c>
       <c r="C32" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="11">
         <v>98.86</v>
       </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13">
+      <c r="E32" s="12">
+        <v>0</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0</v>
+      </c>
+      <c r="G32" s="12">
         <v>4.348</v>
       </c>
     </row>
     <row r="33" ht="20.7" customHeight="1">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>32</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33" s="10">
         <v>3</v>
       </c>
       <c r="C33" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="11">
         <v>98</v>
       </c>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13">
+      <c r="E33" s="12">
+        <v>0</v>
+      </c>
+      <c r="F33" s="12">
+        <v>0</v>
+      </c>
+      <c r="G33" s="12">
         <v>4.274</v>
       </c>
     </row>
     <row r="34" ht="20.7" customHeight="1">
-      <c r="A34" s="10">
+      <c r="A34" s="9">
         <v>33</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34" s="10">
         <v>3</v>
       </c>
       <c r="C34" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="11">
         <v>97.51000000000001</v>
       </c>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13">
+      <c r="E34" s="12">
+        <v>0</v>
+      </c>
+      <c r="F34" s="12">
+        <v>0</v>
+      </c>
+      <c r="G34" s="12">
         <v>4.235</v>
       </c>
     </row>
     <row r="35" ht="20.7" customHeight="1">
-      <c r="A35" s="10">
+      <c r="A35" s="9">
         <v>34</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35" s="10">
         <v>3</v>
       </c>
       <c r="C35" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="11">
         <v>97.70999999999999</v>
       </c>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13">
+      <c r="E35" s="12">
+        <v>0</v>
+      </c>
+      <c r="F35" s="12">
+        <v>0</v>
+      </c>
+      <c r="G35" s="12">
         <v>4.262</v>
       </c>
     </row>
     <row r="36" ht="20.7" customHeight="1">
-      <c r="A36" s="10">
+      <c r="A36" s="9">
         <v>35</v>
       </c>
-      <c r="B36" s="11">
+      <c r="B36" s="10">
         <v>3</v>
       </c>
       <c r="C36" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13"/>
+      <c r="D36" s="11">
+        <v>98.04000000000001</v>
+      </c>
+      <c r="E36" s="16">
+        <v>0</v>
+      </c>
+      <c r="F36" s="15">
+        <v>0</v>
+      </c>
+      <c r="G36" s="11">
+        <v>4.32</v>
+      </c>
     </row>
     <row r="37" ht="20.7" customHeight="1">
-      <c r="A37" s="10">
+      <c r="A37" s="9">
         <v>36</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37" s="10">
         <v>3</v>
       </c>
       <c r="C37" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
+      <c r="D37" s="15">
+        <v>0</v>
+      </c>
+      <c r="E37" s="15">
+        <v>0</v>
+      </c>
+      <c r="F37" s="15">
+        <v>0</v>
+      </c>
+      <c r="G37" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="38" ht="20.7" customHeight="1">
-      <c r="A38" s="10">
+      <c r="A38" s="9">
         <v>37</v>
       </c>
-      <c r="B38" s="11">
+      <c r="B38" s="10">
         <v>4</v>
       </c>
       <c r="C38" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="11">
         <v>95.67</v>
       </c>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13">
+      <c r="E38" s="12">
+        <v>0</v>
+      </c>
+      <c r="F38" s="12">
+        <v>0</v>
+      </c>
+      <c r="G38" s="12">
         <v>3.891</v>
       </c>
     </row>
     <row r="39" ht="20.7" customHeight="1">
-      <c r="A39" s="10">
+      <c r="A39" s="9">
         <v>38</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39" s="10">
         <v>4</v>
       </c>
       <c r="C39" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="11">
         <v>97.01000000000001</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13">
+      <c r="E39" s="12">
+        <v>0</v>
+      </c>
+      <c r="F39" s="12">
+        <v>0</v>
+      </c>
+      <c r="G39" s="12">
         <v>4.04</v>
       </c>
     </row>
     <row r="40" ht="20.7" customHeight="1">
-      <c r="A40" s="10">
+      <c r="A40" s="9">
         <v>39</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40" s="10">
         <v>4</v>
       </c>
       <c r="C40" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="D40" s="12">
+      <c r="D40" s="11">
         <v>99.95</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13">
+      <c r="E40" s="12">
+        <v>0</v>
+      </c>
+      <c r="F40" s="12">
+        <v>0</v>
+      </c>
+      <c r="G40" s="12">
         <v>4.363</v>
       </c>
     </row>
     <row r="41" ht="20.7" customHeight="1">
-      <c r="A41" s="10">
+      <c r="A41" s="9">
         <v>40</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41" s="10">
         <v>4</v>
       </c>
       <c r="C41" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D41" s="12">
+      <c r="D41" s="11">
         <v>100.55</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13">
+      <c r="E41" s="12">
+        <v>0</v>
+      </c>
+      <c r="F41" s="12">
+        <v>0</v>
+      </c>
+      <c r="G41" s="12">
         <v>4.3</v>
       </c>
     </row>
     <row r="42" ht="20.7" customHeight="1">
-      <c r="A42" s="10">
+      <c r="A42" s="9">
         <v>41</v>
       </c>
-      <c r="B42" s="11">
+      <c r="B42" s="10">
         <v>4</v>
       </c>
       <c r="C42" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="D42" s="12">
+      <c r="D42" s="11">
         <v>99.84</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13">
+      <c r="E42" s="12">
+        <v>0</v>
+      </c>
+      <c r="F42" s="12">
+        <v>0</v>
+      </c>
+      <c r="G42" s="12">
         <v>4.092</v>
       </c>
     </row>
     <row r="43" ht="20.7" customHeight="1">
-      <c r="A43" s="10">
+      <c r="A43" s="9">
         <v>42</v>
       </c>
-      <c r="B43" s="11">
+      <c r="B43" s="10">
         <v>4</v>
       </c>
       <c r="C43" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="D43" s="12">
+      <c r="D43" s="11">
         <v>98.70999999999999</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13">
+      <c r="E43" s="12">
+        <v>0</v>
+      </c>
+      <c r="F43" s="12">
+        <v>0</v>
+      </c>
+      <c r="G43" s="12">
         <v>4.078</v>
       </c>
     </row>
     <row r="44" ht="20.7" customHeight="1">
-      <c r="A44" s="10">
+      <c r="A44" s="9">
         <v>43</v>
       </c>
-      <c r="B44" s="11">
+      <c r="B44" s="10">
         <v>4</v>
       </c>
       <c r="C44" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D44" s="12">
+      <c r="D44" s="11">
         <v>98.86</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13">
+      <c r="E44" s="12">
+        <v>0</v>
+      </c>
+      <c r="F44" s="12">
+        <v>0</v>
+      </c>
+      <c r="G44" s="12">
         <v>4.071</v>
       </c>
     </row>
     <row r="45" ht="20.7" customHeight="1">
-      <c r="A45" s="10">
+      <c r="A45" s="9">
         <v>44</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45" s="10">
         <v>4</v>
       </c>
       <c r="C45" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D45" s="12">
+      <c r="D45" s="11">
         <v>98</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13">
+      <c r="E45" s="12">
+        <v>0</v>
+      </c>
+      <c r="F45" s="12">
+        <v>0</v>
+      </c>
+      <c r="G45" s="12">
         <v>4.001</v>
       </c>
     </row>
     <row r="46" ht="20.7" customHeight="1">
-      <c r="A46" s="10">
+      <c r="A46" s="9">
         <v>45</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46" s="10">
         <v>4</v>
       </c>
       <c r="C46" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="D46" s="12">
+      <c r="D46" s="11">
         <v>97.51000000000001</v>
       </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13">
+      <c r="E46" s="12">
+        <v>0</v>
+      </c>
+      <c r="F46" s="12">
+        <v>0</v>
+      </c>
+      <c r="G46" s="12">
         <v>3.965</v>
       </c>
     </row>
     <row r="47" ht="20.7" customHeight="1">
-      <c r="A47" s="10">
+      <c r="A47" s="9">
         <v>46</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47" s="10">
         <v>4</v>
       </c>
       <c r="C47" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D47" s="12">
+      <c r="D47" s="11">
         <v>97.70999999999999</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13">
+      <c r="E47" s="12">
+        <v>0</v>
+      </c>
+      <c r="F47" s="12">
+        <v>0</v>
+      </c>
+      <c r="G47" s="12">
         <v>3.99</v>
       </c>
     </row>
     <row r="48" ht="20.7" customHeight="1">
-      <c r="A48" s="10">
+      <c r="A48" s="9">
         <v>47</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B48" s="10">
         <v>4</v>
       </c>
       <c r="C48" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
+      <c r="D48" s="11">
+        <v>98.04000000000001</v>
+      </c>
+      <c r="E48" s="12">
+        <v>0</v>
+      </c>
+      <c r="F48" s="12">
+        <v>0</v>
+      </c>
+      <c r="G48" s="12">
+        <v>4.05</v>
+      </c>
     </row>
     <row r="49" ht="20.7" customHeight="1">
-      <c r="A49" s="10">
+      <c r="A49" s="9">
         <v>48</v>
       </c>
-      <c r="B49" s="11">
+      <c r="B49" s="10">
         <v>4</v>
       </c>
       <c r="C49" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="D49" s="12"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="D49" s="11">
+        <v>0</v>
+      </c>
+      <c r="E49" s="12">
+        <v>0</v>
+      </c>
+      <c r="F49" s="12">
+        <v>0</v>
+      </c>
+      <c r="G49" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" ht="20.7" customHeight="1">
-      <c r="A50" s="10">
+      <c r="A50" s="9">
         <v>49</v>
       </c>
-      <c r="B50" s="11">
+      <c r="B50" s="10">
         <v>5</v>
       </c>
       <c r="C50" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="D50" s="12">
+      <c r="D50" s="11">
         <v>95.67</v>
       </c>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13">
+      <c r="E50" s="12">
+        <v>0</v>
+      </c>
+      <c r="F50" s="12">
+        <v>0</v>
+      </c>
+      <c r="G50" s="12">
         <v>3.796</v>
       </c>
     </row>
     <row r="51" ht="20.7" customHeight="1">
-      <c r="A51" s="10">
+      <c r="A51" s="9">
         <v>50</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51" s="10">
         <v>5</v>
       </c>
       <c r="C51" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D51" s="12">
+      <c r="D51" s="11">
         <v>97.01000000000001</v>
       </c>
-      <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
-      <c r="G51" s="13">
+      <c r="E51" s="12">
+        <v>0</v>
+      </c>
+      <c r="F51" s="12">
+        <v>0</v>
+      </c>
+      <c r="G51" s="12">
         <v>3.941</v>
       </c>
     </row>
     <row r="52" ht="20.7" customHeight="1">
-      <c r="A52" s="10">
+      <c r="A52" s="9">
         <v>51</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52" s="10">
         <v>5</v>
       </c>
       <c r="C52" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="D52" s="12">
+      <c r="D52" s="11">
         <v>99.95</v>
       </c>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13">
+      <c r="E52" s="12">
+        <v>0</v>
+      </c>
+      <c r="F52" s="12">
+        <v>0</v>
+      </c>
+      <c r="G52" s="12">
         <v>4.256</v>
       </c>
     </row>
     <row r="53" ht="20.7" customHeight="1">
-      <c r="A53" s="10">
+      <c r="A53" s="9">
         <v>52</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53" s="10">
         <v>5</v>
       </c>
       <c r="C53" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D53" s="12">
+      <c r="D53" s="11">
         <v>100.55</v>
       </c>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13">
+      <c r="E53" s="12">
+        <v>0</v>
+      </c>
+      <c r="F53" s="12">
+        <v>0</v>
+      </c>
+      <c r="G53" s="12">
         <v>4.194</v>
       </c>
     </row>
     <row r="54" ht="20.7" customHeight="1">
-      <c r="A54" s="10">
+      <c r="A54" s="9">
         <v>53</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54" s="10">
         <v>5</v>
       </c>
       <c r="C54" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="D54" s="12">
+      <c r="D54" s="11">
         <v>99.84</v>
       </c>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13">
+      <c r="E54" s="12">
+        <v>0</v>
+      </c>
+      <c r="F54" s="12">
+        <v>0</v>
+      </c>
+      <c r="G54" s="12">
         <v>3.991</v>
       </c>
     </row>
     <row r="55" ht="20.7" customHeight="1">
-      <c r="A55" s="10">
+      <c r="A55" s="9">
         <v>54</v>
       </c>
-      <c r="B55" s="11">
+      <c r="B55" s="10">
         <v>5</v>
       </c>
       <c r="C55" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="D55" s="12">
+      <c r="D55" s="11">
         <v>98.70999999999999</v>
       </c>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13">
+      <c r="E55" s="12">
+        <v>0</v>
+      </c>
+      <c r="F55" s="12">
+        <v>0</v>
+      </c>
+      <c r="G55" s="12">
         <v>3.977</v>
       </c>
     </row>
     <row r="56" ht="20.7" customHeight="1">
-      <c r="A56" s="10">
+      <c r="A56" s="9">
         <v>55</v>
       </c>
-      <c r="B56" s="11">
+      <c r="B56" s="10">
         <v>5</v>
       </c>
       <c r="C56" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D56" s="12">
+      <c r="D56" s="11">
         <v>98.86</v>
       </c>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13">
+      <c r="E56" s="12">
+        <v>0</v>
+      </c>
+      <c r="F56" s="12">
+        <v>0</v>
+      </c>
+      <c r="G56" s="12">
         <v>3.971</v>
       </c>
     </row>
     <row r="57" ht="20.7" customHeight="1">
-      <c r="A57" s="10">
+      <c r="A57" s="9">
         <v>56</v>
       </c>
-      <c r="B57" s="11">
+      <c r="B57" s="10">
         <v>5</v>
       </c>
       <c r="C57" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D57" s="12">
+      <c r="D57" s="11">
         <v>98</v>
       </c>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13">
+      <c r="E57" s="12">
+        <v>0</v>
+      </c>
+      <c r="F57" s="12">
+        <v>0</v>
+      </c>
+      <c r="G57" s="12">
         <v>3.903</v>
       </c>
     </row>
     <row r="58" ht="20.7" customHeight="1">
-      <c r="A58" s="10">
+      <c r="A58" s="9">
         <v>57</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B58" s="10">
         <v>5</v>
       </c>
       <c r="C58" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="D58" s="12">
+      <c r="D58" s="11">
         <v>97.51000000000001</v>
       </c>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13">
+      <c r="E58" s="12">
+        <v>0</v>
+      </c>
+      <c r="F58" s="12">
+        <v>0</v>
+      </c>
+      <c r="G58" s="12">
         <v>3.867</v>
       </c>
     </row>
     <row r="59" ht="20.7" customHeight="1">
-      <c r="A59" s="10">
+      <c r="A59" s="9">
         <v>58</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B59" s="10">
         <v>5</v>
       </c>
       <c r="C59" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D59" s="12">
+      <c r="D59" s="11">
         <v>97.70999999999999</v>
       </c>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13">
+      <c r="E59" s="12">
+        <v>0</v>
+      </c>
+      <c r="F59" s="12">
+        <v>0</v>
+      </c>
+      <c r="G59" s="12">
         <v>3.891</v>
       </c>
     </row>
     <row r="60" ht="20.7" customHeight="1">
-      <c r="A60" s="10">
+      <c r="A60" s="9">
         <v>59</v>
       </c>
-      <c r="B60" s="11">
+      <c r="B60" s="10">
         <v>5</v>
       </c>
       <c r="C60" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="D60" s="12"/>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
+      <c r="D60" s="11">
+        <v>98.04000000000001</v>
+      </c>
+      <c r="E60" s="12">
+        <v>0</v>
+      </c>
+      <c r="F60" s="12">
+        <v>0</v>
+      </c>
+      <c r="G60" s="12">
+        <v>3.95</v>
+      </c>
     </row>
     <row r="61" ht="20.7" customHeight="1">
-      <c r="A61" s="10">
+      <c r="A61" s="9">
         <v>60</v>
       </c>
-      <c r="B61" s="11">
+      <c r="B61" s="10">
         <v>5</v>
       </c>
       <c r="C61" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="D61" s="12"/>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
+      <c r="D61" s="11">
+        <v>0</v>
+      </c>
+      <c r="E61" s="12">
+        <v>0</v>
+      </c>
+      <c r="F61" s="12">
+        <v>0</v>
+      </c>
+      <c r="G61" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" ht="20.7" customHeight="1">
-      <c r="A62" s="10">
+      <c r="A62" s="9">
         <v>61</v>
       </c>
-      <c r="B62" s="11">
+      <c r="B62" s="10">
         <v>6</v>
       </c>
       <c r="C62" t="s" s="6">
         <v>7</v>
       </c>
-      <c r="D62" s="12">
+      <c r="D62" s="11">
         <v>95.67</v>
       </c>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13">
+      <c r="E62" s="12">
+        <v>0</v>
+      </c>
+      <c r="F62" s="12">
+        <v>0</v>
+      </c>
+      <c r="G62" s="12">
         <v>3.853</v>
       </c>
     </row>
     <row r="63" ht="20.7" customHeight="1">
-      <c r="A63" s="10">
+      <c r="A63" s="9">
         <v>62</v>
       </c>
-      <c r="B63" s="11">
+      <c r="B63" s="10">
         <v>6</v>
       </c>
       <c r="C63" t="s" s="6">
         <v>8</v>
       </c>
-      <c r="D63" s="12">
+      <c r="D63" s="11">
         <v>97.01000000000001</v>
       </c>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13">
+      <c r="E63" s="12">
+        <v>0</v>
+      </c>
+      <c r="F63" s="12">
+        <v>0</v>
+      </c>
+      <c r="G63" s="12">
         <v>4.001</v>
       </c>
     </row>
     <row r="64" ht="20.7" customHeight="1">
-      <c r="A64" s="10">
+      <c r="A64" s="9">
         <v>63</v>
       </c>
-      <c r="B64" s="11">
+      <c r="B64" s="10">
         <v>6</v>
       </c>
       <c r="C64" t="s" s="6">
         <v>9</v>
       </c>
-      <c r="D64" s="12">
+      <c r="D64" s="11">
         <v>99.95</v>
       </c>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13">
+      <c r="E64" s="12">
+        <v>0</v>
+      </c>
+      <c r="F64" s="12">
+        <v>0</v>
+      </c>
+      <c r="G64" s="12">
         <v>4.321</v>
       </c>
     </row>
     <row r="65" ht="20.7" customHeight="1">
-      <c r="A65" s="10">
+      <c r="A65" s="9">
         <v>64</v>
       </c>
-      <c r="B65" s="11">
+      <c r="B65" s="10">
         <v>6</v>
       </c>
       <c r="C65" t="s" s="6">
         <v>10</v>
       </c>
-      <c r="D65" s="12">
+      <c r="D65" s="11">
         <v>100.55</v>
       </c>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13">
+      <c r="E65" s="12">
+        <v>0</v>
+      </c>
+      <c r="F65" s="12">
+        <v>0</v>
+      </c>
+      <c r="G65" s="12">
         <v>4.258</v>
       </c>
     </row>
     <row r="66" ht="20.7" customHeight="1">
-      <c r="A66" s="10">
+      <c r="A66" s="9">
         <v>65</v>
       </c>
-      <c r="B66" s="11">
+      <c r="B66" s="10">
         <v>6</v>
       </c>
       <c r="C66" t="s" s="6">
         <v>11</v>
       </c>
-      <c r="D66" s="12">
+      <c r="D66" s="11">
         <v>99.84</v>
       </c>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13">
+      <c r="E66" s="12">
+        <v>0</v>
+      </c>
+      <c r="F66" s="12">
+        <v>0</v>
+      </c>
+      <c r="G66" s="12">
         <v>4.052</v>
       </c>
     </row>
     <row r="67" ht="20.7" customHeight="1">
-      <c r="A67" s="10">
+      <c r="A67" s="9">
         <v>66</v>
       </c>
-      <c r="B67" s="11">
+      <c r="B67" s="10">
         <v>6</v>
       </c>
       <c r="C67" t="s" s="6">
         <v>12</v>
       </c>
-      <c r="D67" s="12">
+      <c r="D67" s="11">
         <v>98.70999999999999</v>
       </c>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13">
+      <c r="E67" s="12">
+        <v>0</v>
+      </c>
+      <c r="F67" s="12">
+        <v>0</v>
+      </c>
+      <c r="G67" s="12">
         <v>4.038</v>
       </c>
     </row>
     <row r="68" ht="20.7" customHeight="1">
-      <c r="A68" s="10">
+      <c r="A68" s="9">
         <v>67</v>
       </c>
-      <c r="B68" s="11">
+      <c r="B68" s="10">
         <v>6</v>
       </c>
       <c r="C68" t="s" s="6">
         <v>13</v>
       </c>
-      <c r="D68" s="12">
+      <c r="D68" s="11">
         <v>98.86</v>
       </c>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13">
+      <c r="E68" s="12">
+        <v>0</v>
+      </c>
+      <c r="F68" s="12">
+        <v>0</v>
+      </c>
+      <c r="G68" s="12">
         <v>4.032</v>
       </c>
     </row>
     <row r="69" ht="20.7" customHeight="1">
-      <c r="A69" s="10">
+      <c r="A69" s="9">
         <v>68</v>
       </c>
-      <c r="B69" s="11">
+      <c r="B69" s="10">
         <v>6</v>
       </c>
       <c r="C69" t="s" s="6">
         <v>14</v>
       </c>
-      <c r="D69" s="12">
+      <c r="D69" s="11">
         <v>98</v>
       </c>
-      <c r="E69" s="13"/>
-      <c r="F69" s="13"/>
-      <c r="G69" s="13">
+      <c r="E69" s="12">
+        <v>0</v>
+      </c>
+      <c r="F69" s="12">
+        <v>0</v>
+      </c>
+      <c r="G69" s="12">
         <v>3.963</v>
       </c>
     </row>
     <row r="70" ht="20.7" customHeight="1">
-      <c r="A70" s="10">
+      <c r="A70" s="9">
         <v>69</v>
       </c>
-      <c r="B70" s="11">
+      <c r="B70" s="10">
         <v>6</v>
       </c>
       <c r="C70" t="s" s="6">
         <v>15</v>
       </c>
-      <c r="D70" s="12">
+      <c r="D70" s="11">
         <v>97.51000000000001</v>
       </c>
-      <c r="E70" s="13"/>
-      <c r="F70" s="13"/>
-      <c r="G70" s="13">
+      <c r="E70" s="12">
+        <v>0</v>
+      </c>
+      <c r="F70" s="12">
+        <v>0</v>
+      </c>
+      <c r="G70" s="12">
         <v>3.927</v>
       </c>
     </row>
     <row r="71" ht="20.7" customHeight="1">
-      <c r="A71" s="10">
+      <c r="A71" s="9">
         <v>70</v>
       </c>
-      <c r="B71" s="11">
+      <c r="B71" s="10">
         <v>6</v>
       </c>
       <c r="C71" t="s" s="6">
         <v>16</v>
       </c>
-      <c r="D71" s="12">
+      <c r="D71" s="11">
         <v>97.70999999999999</v>
       </c>
-      <c r="E71" s="13"/>
-      <c r="F71" s="13"/>
-      <c r="G71" s="13">
+      <c r="E71" s="12">
+        <v>0</v>
+      </c>
+      <c r="F71" s="12">
+        <v>0</v>
+      </c>
+      <c r="G71" s="12">
         <v>3.952</v>
       </c>
     </row>
     <row r="72" ht="20.7" customHeight="1">
-      <c r="A72" s="10">
+      <c r="A72" s="9">
         <v>71</v>
       </c>
-      <c r="B72" s="11">
+      <c r="B72" s="10">
         <v>6</v>
       </c>
       <c r="C72" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="D72" s="12"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="13"/>
-      <c r="G72" s="13"/>
+      <c r="D72" s="11">
+        <v>98.04000000000001</v>
+      </c>
+      <c r="E72" s="12">
+        <v>0</v>
+      </c>
+      <c r="F72" s="12">
+        <v>0</v>
+      </c>
+      <c r="G72" s="12">
+        <v>4.01</v>
+      </c>
     </row>
     <row r="73" ht="20.7" customHeight="1">
-      <c r="A73" s="10">
+      <c r="A73" s="9">
         <v>72</v>
       </c>
-      <c r="B73" s="11">
+      <c r="B73" s="10">
         <v>6</v>
       </c>
       <c r="C73" t="s" s="6">
         <v>18</v>
       </c>
-      <c r="D73" s="12"/>
-      <c r="E73" s="13"/>
-      <c r="F73" s="13"/>
-      <c r="G73" s="13"/>
+      <c r="D73" s="11">
+        <v>0</v>
+      </c>
+      <c r="E73" s="12">
+        <v>0</v>
+      </c>
+      <c r="F73" s="12">
+        <v>0</v>
+      </c>
+      <c r="G73" s="12">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>

<commit_message>
modified update for next records and modified view by history
</commit_message>
<xml_diff>
--- a/easylight/doc/Tarifa_Alto_Consumo.xlsx
+++ b/easylight/doc/Tarifa_Alto_Consumo.xlsx
@@ -1687,14 +1687,14 @@
       <c r="C13" t="s" s="6">
         <v>17</v>
       </c>
-      <c r="D13" s="11">
-        <v>0</v>
+      <c r="D13" s="13">
+        <v>98.04000000000001</v>
       </c>
       <c r="E13" s="12">
-        <v>0</v>
-      </c>
-      <c r="F13" s="12">
-        <v>0</v>
+        <v>4.201</v>
+      </c>
+      <c r="F13" s="14">
+        <v>3.61</v>
       </c>
     </row>
     <row r="14" ht="20.7" customHeight="1">
@@ -1928,13 +1928,13 @@
         <v>17</v>
       </c>
       <c r="D25" s="15">
-        <v>0</v>
-      </c>
-      <c r="E25" s="15">
-        <v>0</v>
-      </c>
-      <c r="F25" s="11">
-        <v>0</v>
+        <v>98.04000000000001</v>
+      </c>
+      <c r="E25" s="11">
+        <v>4.58</v>
+      </c>
+      <c r="F25" s="12">
+        <v>3.61</v>
       </c>
     </row>
     <row r="26" ht="20.7" customHeight="1">
@@ -2168,13 +2168,13 @@
         <v>17</v>
       </c>
       <c r="D37" s="15">
-        <v>0</v>
+        <v>98.04000000000001</v>
       </c>
       <c r="E37" s="15">
-        <v>0</v>
+        <v>4.32</v>
       </c>
       <c r="F37" s="11">
-        <v>0</v>
+        <v>4.32</v>
       </c>
     </row>
     <row r="38" ht="20.7" customHeight="1">
@@ -2408,13 +2408,13 @@
         <v>17</v>
       </c>
       <c r="D49" s="11">
-        <v>0</v>
+        <v>98.04000000000001</v>
       </c>
       <c r="E49" s="12">
-        <v>0</v>
+        <v>4.05</v>
       </c>
       <c r="F49" s="12">
-        <v>0</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="50" ht="20.7" customHeight="1">
@@ -2648,13 +2648,13 @@
         <v>17</v>
       </c>
       <c r="D61" s="11">
-        <v>0</v>
+        <v>98.04000000000001</v>
       </c>
       <c r="E61" s="12">
-        <v>0</v>
+        <v>3.95</v>
       </c>
       <c r="F61" s="12">
-        <v>0</v>
+        <v>3.95</v>
       </c>
     </row>
     <row r="62" ht="20.7" customHeight="1">
@@ -2888,13 +2888,13 @@
         <v>17</v>
       </c>
       <c r="D73" s="11">
-        <v>0</v>
+        <v>98.04000000000001</v>
       </c>
       <c r="E73" s="12">
-        <v>0</v>
+        <v>4.01</v>
       </c>
       <c r="F73" s="12">
-        <v>0</v>
+        <v>4.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>